<commit_message>
feat: populate travel request template
</commit_message>
<xml_diff>
--- a/templates/travel_request_template.xlsx
+++ b/templates/travel_request_template.xlsx
@@ -413,14 +413,192 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Travel Request Template (ITIN-2025.1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>&lt;&lt;traveler_name&gt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>&lt;&lt;business_purpose&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>&lt;&lt;cost_center&gt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>&lt;&lt;city_state&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>&lt;&lt;destination_zip&gt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>&lt;&lt;depart_date&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>&lt;&lt;return_date&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>&lt;&lt;event_registration_cost&gt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>&lt;&lt;flight_pref_outbound.carrier_flight&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>&lt;&lt;flight_pref_outbound.depart_time&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>&lt;&lt;flight_pref_outbound.arrive_time&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>&lt;&lt;flight_pref_outbound.roundtrip_cost&gt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>&lt;&lt;flight_pref_return.carrier_flight&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>&lt;&lt;flight_pref_return.depart_time&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>&lt;&lt;flight_pref_return.arrive_time&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>&lt;&lt;lowest_cost_roundtrip&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>&lt;&lt;parking_estimate&gt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>&lt;&lt;hotel.name&gt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>&lt;&lt;hotel.address&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>&lt;&lt;hotel.city_state&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>&lt;&lt;hotel.nightly_rate&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>&lt;&lt;hotel.nights&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>&lt;&lt;hotel.conference_hotel&gt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>&lt;&lt;hotel.price_compare_notes&gt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>&lt;&lt;comparable_hotels[0].name&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>&lt;&lt;comparable_hotels[0].nightly_rate&gt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>&lt;&lt;ground_transport_pref&gt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>&lt;&lt;notes&gt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="H20">
+        <f>SUM(H15:H19)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore(codex): bootstrap PR for issue #105 (#121)
* chore(codex): bootstrap PR for issue #105

* Align template mapping with asset

* chore(codex-keepalive): apply updates (PR #121)

* feat: populate travel request template

* chore(codex-keepalive): apply updates (PR #121)

---------

Co-authored-by: github-actions[bot] <github-actions[bot]@users.noreply.github.com>
Co-authored-by: codex <codex@example.com>
Co-authored-by: github-actions[bot] <41898282+github-actions[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/templates/travel_request_template.xlsx
+++ b/templates/travel_request_template.xlsx
@@ -413,14 +413,192 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Travel Request Template (ITIN-2025.1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>&lt;&lt;traveler_name&gt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>&lt;&lt;business_purpose&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>&lt;&lt;cost_center&gt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>&lt;&lt;city_state&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>&lt;&lt;destination_zip&gt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>&lt;&lt;depart_date&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>&lt;&lt;return_date&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>&lt;&lt;event_registration_cost&gt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>&lt;&lt;flight_pref_outbound.carrier_flight&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>&lt;&lt;flight_pref_outbound.depart_time&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>&lt;&lt;flight_pref_outbound.arrive_time&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>&lt;&lt;flight_pref_outbound.roundtrip_cost&gt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>&lt;&lt;flight_pref_return.carrier_flight&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>&lt;&lt;flight_pref_return.depart_time&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>&lt;&lt;flight_pref_return.arrive_time&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>&lt;&lt;lowest_cost_roundtrip&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>&lt;&lt;parking_estimate&gt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>&lt;&lt;hotel.name&gt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>&lt;&lt;hotel.address&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>&lt;&lt;hotel.city_state&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>&lt;&lt;hotel.nightly_rate&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>&lt;&lt;hotel.nights&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>&lt;&lt;hotel.conference_hotel&gt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>&lt;&lt;hotel.price_compare_notes&gt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>&lt;&lt;comparable_hotels[0].name&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>&lt;&lt;comparable_hotels[0].nightly_rate&gt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>&lt;&lt;ground_transport_pref&gt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>&lt;&lt;notes&gt;&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="H20">
+        <f>SUM(H15:H19)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>